<commit_message>
Feat- update otdr dan RFS
Feat- update otdr
</commit_message>
<xml_diff>
--- a/cypress/downloads/resultsApproval_NewBuildMacro.xlsx
+++ b/cypress/downloads/resultsApproval_NewBuildMacro.xlsx
@@ -424,7 +424,7 @@
         <v>Pass</v>
       </c>
       <c r="C2" t="str">
-        <v>2025-02-25T03:56:03.192Z</v>
+        <v>2025-02-27T07:04:28.053Z</v>
       </c>
     </row>
     <row r="3">
@@ -435,7 +435,7 @@
         <v>Pass</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-02-25T03:56:14.295Z</v>
+        <v>2025-02-27T07:04:39.503Z</v>
       </c>
     </row>
     <row r="4">
@@ -446,7 +446,7 @@
         <v>Pass</v>
       </c>
       <c r="D4" t="str">
-        <v>2025-02-25T03:56:15.948Z</v>
+        <v>2025-02-27T07:04:40.609Z</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat-update dynamic link SIT
feat-update dynamic link SIT
</commit_message>
<xml_diff>
--- a/cypress/downloads/resultsApproval_NewBuildMacro.xlsx
+++ b/cypress/downloads/resultsApproval_NewBuildMacro.xlsx
@@ -424,7 +424,7 @@
         <v>Pass</v>
       </c>
       <c r="C2" t="str">
-        <v>2025-02-28T09:06:44.844Z</v>
+        <v>2025-03-02T21:13:03.249Z</v>
       </c>
     </row>
     <row r="3">
@@ -435,7 +435,7 @@
         <v>Pass</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-02-28T09:06:55.062Z</v>
+        <v>2025-03-02T21:13:13.304Z</v>
       </c>
     </row>
     <row r="4">
@@ -446,7 +446,7 @@
         <v>Pass</v>
       </c>
       <c r="D4" t="str">
-        <v>2025-02-28T09:06:55.504Z</v>
+        <v>2025-03-02T21:13:14.450Z</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat- pecah project dan asset
feat- pecah project dan asset
</commit_message>
<xml_diff>
--- a/cypress/downloads/resultsApproval_NewBuildMacro.xlsx
+++ b/cypress/downloads/resultsApproval_NewBuildMacro.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -410,48 +410,56 @@
         <v>Status</v>
       </c>
       <c r="C1" t="str">
-        <v>timeStamp</v>
-      </c>
-      <c r="D1" t="str">
         <v>Timestamp</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>User PM FO melakukan akses ke menu Project activity Header</v>
+        <v>Button Clicked</v>
       </c>
       <c r="B2" t="str">
         <v>Pass</v>
       </c>
       <c r="C2" t="str">
-        <v>2025-12-15T07:08:40.947Z</v>
+        <v>2025-12-17T06:43:14.512Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>User AM melakukan klik tombol Search di Stip approval</v>
+        <v>User masuk ke Page PV Master List Maintenance</v>
       </c>
       <c r="B3" t="str">
         <v>Pass</v>
       </c>
-      <c r="D3" t="str">
-        <v>2025-12-15T07:08:52.197Z</v>
+      <c r="C3" t="str">
+        <v>2025-12-17T06:43:14.513Z</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>User AM melakukan klik tombol Search di Stip approval</v>
+        <v>User ID Input</v>
       </c>
       <c r="B4" t="str">
         <v>Pass</v>
       </c>
-      <c r="D4" t="str">
-        <v>2025-12-15T07:08:54.988Z</v>
+      <c r="C4" t="str">
+        <v>2025-12-17T06:43:15.068Z</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Password has been inputed</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2025-12-17T06:43:15.314Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>